<commit_message>
Multi sheet importer (parser) v.0.9.
</commit_message>
<xml_diff>
--- a/src/test/resources/Basic_data.xlsx
+++ b/src/test/resources/Basic_data.xlsx
@@ -13,15 +13,16 @@
   </bookViews>
   <sheets>
     <sheet name="Basic_chains" sheetId="11" r:id="rId1"/>
-    <sheet name="Basic_categories " sheetId="12" r:id="rId2"/>
-    <sheet name="Basic_action_types" sheetId="13" r:id="rId3"/>
+    <sheet name="Basic_categories" sheetId="12" r:id="rId2"/>
+    <sheet name="Basic_subcategories" sheetId="14" r:id="rId3"/>
+    <sheet name="Basic_action_types" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>Торговая сеть</t>
   </si>
@@ -120,6 +121,111 @@
   </si>
   <si>
     <t>1+1</t>
+  </si>
+  <si>
+    <t>Хлебобулочные изделия</t>
+  </si>
+  <si>
+    <t>Сдобные изделия</t>
+  </si>
+  <si>
+    <t>Хлеб, батон</t>
+  </si>
+  <si>
+    <t>Хлебцы</t>
+  </si>
+  <si>
+    <t>Овощи и фрукты</t>
+  </si>
+  <si>
+    <t>Грибы</t>
+  </si>
+  <si>
+    <t>Овощи</t>
+  </si>
+  <si>
+    <t>Фрукты</t>
+  </si>
+  <si>
+    <t>Ягоды</t>
+  </si>
+  <si>
+    <t>Молочные продукты, яйца</t>
+  </si>
+  <si>
+    <t>Мясо и колбасные изделия</t>
+  </si>
+  <si>
+    <t>Напитки, кофе, чай, соки</t>
+  </si>
+  <si>
+    <t>Бакалея</t>
+  </si>
+  <si>
+    <t>Рыба и морепродукты</t>
+  </si>
+  <si>
+    <t>Сладости</t>
+  </si>
+  <si>
+    <t>Замороженные продукты</t>
+  </si>
+  <si>
+    <t>Детское питание</t>
+  </si>
+  <si>
+    <t>Собственное производство</t>
+  </si>
+  <si>
+    <t>Кисломолочные изделия</t>
+  </si>
+  <si>
+    <t>Масло</t>
+  </si>
+  <si>
+    <t>Молоко</t>
+  </si>
+  <si>
+    <t>Мороженое</t>
+  </si>
+  <si>
+    <t>Сметана</t>
+  </si>
+  <si>
+    <t>Сыр</t>
+  </si>
+  <si>
+    <t>Творожные продукты</t>
+  </si>
+  <si>
+    <t>Яйцо</t>
+  </si>
+  <si>
+    <t>Синоним</t>
+  </si>
+  <si>
+    <t>bel-market</t>
+  </si>
+  <si>
+    <t>prostore</t>
+  </si>
+  <si>
+    <t>rublevski</t>
+  </si>
+  <si>
+    <t>sosedi</t>
+  </si>
+  <si>
+    <t>vitalur</t>
+  </si>
+  <si>
+    <t>evroopt</t>
+  </si>
+  <si>
+    <t>korona</t>
+  </si>
+  <si>
+    <t>almi</t>
   </si>
 </sst>
 </file>
@@ -148,7 +254,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +264,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,43 +287,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,127 +623,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="24.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="18" style="9" customWidth="1"/>
+    <col min="1" max="4" width="15.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>23</v>
+      <c r="C9" s="20"/>
+      <c r="D9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -636,53 +780,428 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="5" customWidth="1"/>
-    <col min="3" max="5" width="18" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="4" width="15.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9">
+        <v>100</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10">
+        <v>200</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10">
+        <v>300</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="10">
+        <v>400</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="10">
+        <v>700</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="10">
+        <v>500</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="10">
+        <v>600</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="10">
+        <v>900</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="10">
+        <v>800</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1100</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="4" width="15.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>26</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="11">
+        <v>400</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="11">
+        <v>600</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="11">
+        <v>800</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="11">
+        <v>500</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="11">
+        <v>200</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="11">
+        <v>300</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="11">
+        <v>700</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="11">
+        <v>200</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="11">
+        <v>300</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="11">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="11">
+        <v>200</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="11">
+        <v>400</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="11">
+        <v>300</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="11">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -690,44 +1209,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18" style="5" customWidth="1"/>
+    <col min="1" max="2" width="18" style="2" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>